<commit_message>
sửa lại phần xem thông tin về sách của thủ thư Module 15 bi delete
</commit_message>
<xml_diff>
--- a/BaoCaoNhom/Project Description.xlsx
+++ b/BaoCaoNhom/Project Description.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="123820"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225"/>
+    <workbookView xWindow="240" yWindow="180" windowWidth="14940" windowHeight="9165"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
   <si>
     <t>Thay đổi thông tin sách, có khả năng thay đổi toàn bộ thông tin về sách</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Thông tin thêm về sách khi sách được đưa ra cho mượn online</t>
   </si>
   <si>
-    <t>2. Trạng thái của sách khi được trả lại thư viện</t>
-  </si>
-  <si>
     <t>Đăng ký mượn sách/hủy mượn sách</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
     <t>Hỗ trợ đa ngôn ngữ</t>
   </si>
   <si>
-    <t>15.</t>
-  </si>
-  <si>
     <t>8.</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
   </si>
   <si>
     <t>3.</t>
-  </si>
-  <si>
-    <t>16.</t>
   </si>
   <si>
     <t>1. Hỗ trợ gửi mail khi người dùng tạo tài khoản mới</t>
@@ -141,9 +132,6 @@
   </si>
   <si>
     <t>10.</t>
-  </si>
-  <si>
-    <t>3. Số lượng hiện tại của 1 loại sách còn lại trong kho</t>
   </si>
   <si>
     <t>Log in / out user</t>
@@ -187,9 +175,6 @@
 14. Ký hiệu xếp giá</t>
   </si>
   <si>
-    <t>1. Danh sách các sách đã trả trong tuần/tháng</t>
-  </si>
-  <si>
     <t>1. Tạo một trang HTML với một số form để user điền vào</t>
   </si>
   <si>
@@ -288,9 +273,6 @@
   </si>
   <si>
     <t>14.</t>
-  </si>
-  <si>
-    <t>Thủ thư xem thông tin về sách mượn và trả của người dùng</t>
   </si>
   <si>
     <t>2. Tăng cuốn sách có thể mượn của user lên 1</t>
@@ -423,7 +405,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -453,6 +435,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -827,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -842,7 +827,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -866,137 +851,137 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="89.25" x14ac:dyDescent="0.2">
       <c r="C6" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C8" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="63.75" x14ac:dyDescent="0.2">
       <c r="C9" s="5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="140.25" x14ac:dyDescent="0.2">
       <c r="C10" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C12" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C13" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C15" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C16" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="178.5" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
@@ -1004,41 +989,41 @@
         <v>3</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C23" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C24" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
@@ -1048,110 +1033,110 @@
     </row>
     <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C28" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C30" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C31" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C32" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C33" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C35" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C37" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C38" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C39" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C41" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C42" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1161,168 +1146,143 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C46" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C47" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B49" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C50" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C51" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B52" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C53" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C54" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C56" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C57" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="10">
+        <v>15</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C59" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C60" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C61" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C63" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C64" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C65" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C66" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
+    <row r="62" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C62" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="67" spans="5:20" x14ac:dyDescent="0.2">
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -1340,17 +1300,17 @@
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
     </row>
-    <row r="70" spans="1:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="1:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="1:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="1:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="1:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="1:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="1:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="5:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="5:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="5:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="5:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="5:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="5:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="5:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="5:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="5:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="5:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="5:20" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>